<commit_message>
Version 2: Added test cases, comments, and finalized all modules
</commit_message>
<xml_diff>
--- a/converting-test-cases.xlsx
+++ b/converting-test-cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\CPR101-NCC\FinalProjV1\Group33_Version01\converting_module\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\CPR101-NCC\Group33_FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11832C61-0F79-42AA-BA1A-8C61875C4884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1FE0D1-CF98-4A67-9429-D958FF2EB5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -278,7 +278,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{F73B17DE-5D6D-4BEE-8A16-22F591181658}">
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{F73B17DE-5D6D-4BEE-8A16-22F591181658}">
       <text>
         <r>
           <rPr>
@@ -322,7 +322,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{F368EADF-F05B-4C15-A4E0-CA9F2F783275}">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{F368EADF-F05B-4C15-A4E0-CA9F2F783275}">
       <text>
         <r>
           <rPr>
@@ -387,7 +387,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{89399E78-2781-46CB-8982-30E3233EC7BC}">
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{89399E78-2781-46CB-8982-30E3233EC7BC}">
       <text>
         <r>
           <rPr>
@@ -413,7 +413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{34FB52D3-7A1D-4C5B-9838-1E77E035A0FA}">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{34FB52D3-7A1D-4C5B-9838-1E77E035A0FA}">
       <text>
         <r>
           <rPr>
@@ -458,7 +458,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{400DA026-3EB6-4927-87CA-8598E92E8996}">
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{400DA026-3EB6-4927-87CA-8598E92E8996}">
       <text>
         <r>
           <rPr>
@@ -482,7 +482,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{9E419422-AFBA-4A9D-AF8D-AF50B3D1D5D0}">
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{9E419422-AFBA-4A9D-AF8D-AF50B3D1D5D0}">
       <text>
         <r>
           <rPr>
@@ -505,7 +505,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{99451D2F-B00E-4B10-92E4-565F887D03DF}">
+    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{99451D2F-B00E-4B10-92E4-565F887D03DF}">
       <text>
         <r>
           <rPr>
@@ -520,7 +520,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{C02017E4-821F-4A2D-86D8-AB6EEDB22A86}">
+    <comment ref="A21" authorId="0" shapeId="0" xr:uid="{C02017E4-821F-4A2D-86D8-AB6EEDB22A86}">
       <text>
         <r>
           <rPr>
@@ -564,7 +564,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{05B2FD82-D89E-4CA6-B9CD-DADA87D3459D}">
+    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{05B2FD82-D89E-4CA6-B9CD-DADA87D3459D}">
       <text>
         <r>
           <rPr>
@@ -629,7 +629,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{23C8660F-F760-4D26-A851-EB73153BFF94}">
+    <comment ref="C21" authorId="0" shapeId="0" xr:uid="{23C8660F-F760-4D26-A851-EB73153BFF94}">
       <text>
         <r>
           <rPr>
@@ -655,7 +655,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{D011BF0E-2314-4932-9D14-810DC408E97A}">
+    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{D011BF0E-2314-4932-9D14-810DC408E97A}">
       <text>
         <r>
           <rPr>
@@ -700,7 +700,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E19" authorId="0" shapeId="0" xr:uid="{135F8B3A-CCD4-4CA6-9ADB-2D061B1E1D5D}">
+    <comment ref="E21" authorId="0" shapeId="0" xr:uid="{135F8B3A-CCD4-4CA6-9ADB-2D061B1E1D5D}">
       <text>
         <r>
           <rPr>
@@ -724,7 +724,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{CDD09690-9535-4ED1-A265-0F0404D34131}">
+    <comment ref="F21" authorId="0" shapeId="0" xr:uid="{CDD09690-9535-4ED1-A265-0F0404D34131}">
       <text>
         <r>
           <rPr>
@@ -747,7 +747,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{508032F0-07F6-4EDA-A011-0A700A6AF801}">
+    <comment ref="G21" authorId="0" shapeId="0" xr:uid="{508032F0-07F6-4EDA-A011-0A700A6AF801}">
       <text>
         <r>
           <rPr>
@@ -767,7 +767,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="67">
   <si>
     <t>Comments</t>
   </si>
@@ -927,6 +927,73 @@
   </si>
   <si>
     <t>Recommended fix: Add logic to detect overflow before using atoi().</t>
+  </si>
+  <si>
+    <t>Michaela Cruz
+November 30, 2024</t>
+  </si>
+  <si>
+    <t>Validate valid double conversion</t>
+  </si>
+  <si>
+    <t>Validate negative double conversion</t>
+  </si>
+  <si>
+    <t>Validate conversion of float-like double string</t>
+  </si>
+  <si>
+    <t>Validate valid integer conversion (conversion to double)</t>
+  </si>
+  <si>
+    <t>Validate handling of valid input with leading spaces</t>
+  </si>
+  <si>
+    <t>- Ensure empty string is handled gracefully</t>
+  </si>
+  <si>
+    <t>+ Ensure valid input with leading/trailing spaces is handled correctly</t>
+  </si>
+  <si>
+    <t>+ Ensure correct conversion of valid integer string</t>
+  </si>
+  <si>
+    <t>+ Ensure correct conversion when input is a float-like string</t>
+  </si>
+  <si>
+    <t>+ Ensure correct conversion of negative double string input</t>
+  </si>
+  <si>
+    <t>+ Ensure correct conversion of valid double string input</t>
+  </si>
+  <si>
+    <t>string: "-123.456"</t>
+  </si>
+  <si>
+    <t>Converts to double: -123.456 and prints "Converted number is -123.456"</t>
+  </si>
+  <si>
+    <t>Converts to double: 4.9089 and prints "Converted number is 4.908900"</t>
+  </si>
+  <si>
+    <t>Converts to double: 101 and prints "Converted number is 101.000000"</t>
+  </si>
+  <si>
+    <t>Program should either handle the empty string gracefully or prompt the user to enter a valid value</t>
+  </si>
+  <si>
+    <t>Recommended fix: Adjust the code to check for empty string and prompt user instead of processing as 0.</t>
+  </si>
+  <si>
+    <t>string: "654.321"</t>
+  </si>
+  <si>
+    <t>Converts to double: 654.321 and prints "Converted number is 654.321"</t>
+  </si>
+  <si>
+    <t>string: " 600 "</t>
+  </si>
+  <si>
+    <t>Converts to double: 600 and prints "Converted number is 800.000000"</t>
   </si>
 </sst>
 </file>
@@ -1200,7 +1267,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1273,6 +1340,12 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1578,10 +1651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489FCF92-76BB-4101-9D49-11677A4362B7}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1771,129 +1844,208 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="4" t="s">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G11" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="50" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="50" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="50" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="25"/>
+    </row>
+    <row r="20" spans="1:7" ht="26.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="26.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+    <row r="21" spans="1:7" ht="26.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B21" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C21" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D21" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E21" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F21" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G21" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="9"/>
-    </row>
-    <row r="17" spans="1:7" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="9"/>
-    </row>
-    <row r="18" spans="1:7" ht="26.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="26.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="9"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="9"/>
     </row>
     <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
@@ -1937,11 +2089,23 @@
       <c r="E28" s="2"/>
       <c r="F28" s="9"/>
     </row>
+    <row r="29" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="13"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="13"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A20:E20"/>
     <mergeCell ref="C1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F1048576">

</xml_diff>